<commit_message>
Update Tracking Use Case - Robust Analisis (Module GLIK).xlsx
</commit_message>
<xml_diff>
--- a/Robust Analisis - Likuidasi/Tracking Use Case - Robust Analisis (Module GLIK).xlsx
+++ b/Robust Analisis - Likuidasi/Tracking Use Case - Robust Analisis (Module GLIK).xlsx
@@ -8,20 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toshiba\Documents\GitHub\GLIK-DM\Robust Analisis - Likuidasi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1CC510-CA6E-4CD0-AAC2-39EE3C8A2628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEF08DE-180E-4B07-A3FB-23502339EA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{9D093FFE-4593-44B8-843D-58E930F801B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Use Case - Persiapan" sheetId="2" r:id="rId1"/>
-    <sheet name="Traciking - Pengawasan (TSD)" sheetId="7" r:id="rId2"/>
+    <sheet name="TSD - Pengawasan" sheetId="8" r:id="rId2"/>
     <sheet name="Use Case - Pengawasan" sheetId="1" r:id="rId3"/>
     <sheet name="Use Case - Pengakhiran" sheetId="4" r:id="rId4"/>
     <sheet name="Aplikasi Tim Likuidasi" sheetId="6" r:id="rId5"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Traciking - Pengawasan (TSD)'!$C$3:$C$67</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="319">
   <si>
     <t>Nama Use Case</t>
   </si>
@@ -1114,7 +1111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1213,9 +1210,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1242,6 +1236,12 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1249,12 +1249,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1631,10 +1625,10 @@
       <c r="B3" s="11">
         <v>1</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="50" t="s">
         <v>159</v>
       </c>
       <c r="E3" s="26" t="s">
@@ -1648,7 +1642,7 @@
         <v>256</v>
       </c>
       <c r="I3" s="33"/>
-      <c r="J3" s="51" t="s">
+      <c r="J3" s="52" t="s">
         <v>94</v>
       </c>
       <c r="K3" s="26" t="s">
@@ -1662,8 +1656,8 @@
       <c r="B4" s="11">
         <v>2</v>
       </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
       <c r="E4" s="26" t="s">
         <v>139</v>
       </c>
@@ -1675,7 +1669,7 @@
         <v>256</v>
       </c>
       <c r="I4" s="33"/>
-      <c r="J4" s="51"/>
+      <c r="J4" s="52"/>
       <c r="K4" s="26" t="s">
         <v>263</v>
       </c>
@@ -1687,8 +1681,8 @@
       <c r="B5" s="11">
         <v>3</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
       <c r="E5" s="26" t="s">
         <v>140</v>
       </c>
@@ -1700,7 +1694,7 @@
         <v>256</v>
       </c>
       <c r="I5" s="33"/>
-      <c r="J5" s="51"/>
+      <c r="J5" s="52"/>
       <c r="K5" s="26" t="s">
         <v>265</v>
       </c>
@@ -1712,8 +1706,8 @@
       <c r="B6" s="11">
         <v>4</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
       <c r="E6" s="26" t="s">
         <v>141</v>
       </c>
@@ -1727,7 +1721,7 @@
         <v>300</v>
       </c>
       <c r="I6" s="33"/>
-      <c r="J6" s="51"/>
+      <c r="J6" s="52"/>
       <c r="K6" s="26" t="s">
         <v>267</v>
       </c>
@@ -1739,8 +1733,8 @@
       <c r="B7" s="11">
         <v>5</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
       <c r="E7" s="26" t="s">
         <v>142</v>
       </c>
@@ -1752,7 +1746,7 @@
         <v>256</v>
       </c>
       <c r="I7" s="33"/>
-      <c r="J7" s="51"/>
+      <c r="J7" s="52"/>
       <c r="K7" s="26" t="s">
         <v>269</v>
       </c>
@@ -1764,8 +1758,8 @@
       <c r="B8" s="11">
         <v>6</v>
       </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
       <c r="E8" s="26" t="s">
         <v>143</v>
       </c>
@@ -1777,7 +1771,7 @@
         <v>256</v>
       </c>
       <c r="I8" s="33"/>
-      <c r="J8" s="51"/>
+      <c r="J8" s="52"/>
       <c r="K8" s="26" t="s">
         <v>271</v>
       </c>
@@ -1789,8 +1783,8 @@
       <c r="B9" s="11">
         <v>7</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
       <c r="E9" s="26" t="s">
         <v>144</v>
       </c>
@@ -1802,7 +1796,7 @@
         <v>256</v>
       </c>
       <c r="I9" s="33"/>
-      <c r="J9" s="51"/>
+      <c r="J9" s="52"/>
       <c r="K9" s="26" t="s">
         <v>273</v>
       </c>
@@ -1814,8 +1808,8 @@
       <c r="B10" s="11">
         <v>8</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
       <c r="E10" s="26" t="s">
         <v>145</v>
       </c>
@@ -1827,7 +1821,7 @@
         <v>256</v>
       </c>
       <c r="I10" s="33"/>
-      <c r="J10" s="51"/>
+      <c r="J10" s="52"/>
       <c r="K10" s="26" t="s">
         <v>275</v>
       </c>
@@ -1839,8 +1833,8 @@
       <c r="B11" s="11">
         <v>9</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
       <c r="E11" s="26" t="s">
         <v>146</v>
       </c>
@@ -1852,7 +1846,7 @@
         <v>256</v>
       </c>
       <c r="I11" s="33"/>
-      <c r="J11" s="51"/>
+      <c r="J11" s="52"/>
       <c r="K11" s="26" t="s">
         <v>277</v>
       </c>
@@ -1864,8 +1858,8 @@
       <c r="B12" s="11">
         <v>10</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
       <c r="E12" s="26" t="s">
         <v>147</v>
       </c>
@@ -1877,7 +1871,7 @@
         <v>257</v>
       </c>
       <c r="I12" s="33"/>
-      <c r="J12" s="51"/>
+      <c r="J12" s="52"/>
       <c r="K12" s="26" t="s">
         <v>279</v>
       </c>
@@ -1889,8 +1883,8 @@
       <c r="B13" s="11">
         <v>11</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
       <c r="E13" s="26" t="s">
         <v>148</v>
       </c>
@@ -1902,7 +1896,7 @@
         <v>257</v>
       </c>
       <c r="I13" s="33"/>
-      <c r="J13" s="51"/>
+      <c r="J13" s="52"/>
       <c r="K13" s="26" t="s">
         <v>279</v>
       </c>
@@ -1914,8 +1908,8 @@
       <c r="B14" s="11">
         <v>12</v>
       </c>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
       <c r="E14" s="26" t="s">
         <v>149</v>
       </c>
@@ -1927,7 +1921,7 @@
         <v>257</v>
       </c>
       <c r="I14" s="33"/>
-      <c r="J14" s="50" t="s">
+      <c r="J14" s="51" t="s">
         <v>155</v>
       </c>
       <c r="K14" s="26" t="s">
@@ -1941,8 +1935,8 @@
       <c r="B15" s="11">
         <v>13</v>
       </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
       <c r="E15" s="26" t="s">
         <v>150</v>
       </c>
@@ -1954,7 +1948,7 @@
         <v>257</v>
       </c>
       <c r="I15" s="33"/>
-      <c r="J15" s="50"/>
+      <c r="J15" s="51"/>
       <c r="K15" s="26" t="s">
         <v>279</v>
       </c>
@@ -1969,7 +1963,7 @@
       <c r="C16" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="D16" s="49"/>
+      <c r="D16" s="50"/>
       <c r="E16" s="26" t="s">
         <v>153</v>
       </c>
@@ -1982,7 +1976,7 @@
       <c r="H16" s="32" t="s">
         <v>300</v>
       </c>
-      <c r="J16" s="50"/>
+      <c r="J16" s="51"/>
       <c r="K16" s="26" t="s">
         <v>280</v>
       </c>
@@ -1994,10 +1988,10 @@
       <c r="B17" s="11">
         <v>15</v>
       </c>
-      <c r="C17" s="50" t="s">
+      <c r="C17" s="51" t="s">
         <v>155</v>
       </c>
-      <c r="D17" s="49"/>
+      <c r="D17" s="50"/>
       <c r="E17" s="26" t="s">
         <v>156</v>
       </c>
@@ -2009,7 +2003,7 @@
         <v>257</v>
       </c>
       <c r="I17" s="33"/>
-      <c r="J17" s="50"/>
+      <c r="J17" s="51"/>
       <c r="K17" s="26" t="s">
         <v>282</v>
       </c>
@@ -2021,8 +2015,8 @@
       <c r="B18" s="11">
         <v>16</v>
       </c>
-      <c r="C18" s="50"/>
-      <c r="D18" s="49"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="50"/>
       <c r="E18" s="26" t="s">
         <v>157</v>
       </c>
@@ -2048,8 +2042,8 @@
       <c r="B19" s="11">
         <v>17</v>
       </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="49"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="50"/>
       <c r="E19" s="26" t="s">
         <v>158</v>
       </c>
@@ -2069,8 +2063,8 @@
       <c r="B20" s="11">
         <v>18</v>
       </c>
-      <c r="C20" s="50"/>
-      <c r="D20" s="49"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="50"/>
       <c r="E20" s="26" t="s">
         <v>149</v>
       </c>
@@ -2090,8 +2084,8 @@
       <c r="B21" s="11">
         <v>19</v>
       </c>
-      <c r="C21" s="50"/>
-      <c r="D21" s="49"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="50"/>
       <c r="E21" s="26" t="s">
         <v>150</v>
       </c>
@@ -2122,1371 +2116,1439 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A65867-F2EE-4131-9D22-05A2B26DC5E8}">
-  <dimension ref="B2:J67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB03414-4B51-4449-A50A-AD9A95CAA7B7}">
+  <dimension ref="B2:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="2.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.26953125" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.90625" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7265625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="49" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" style="49" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="65" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.90625" style="49" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7265625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9">
+    <row r="2" spans="2:10">
       <c r="B2" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="E2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>298</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="G2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="H2" s="13" t="s">
         <v>301</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="I2" s="13" t="s">
         <v>299</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="J2" s="13" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="3" spans="2:9">
+    <row r="3" spans="2:10">
       <c r="B3" s="31">
         <v>1</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="E3" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G3" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="G3" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H3" s="47"/>
-      <c r="I3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9">
+      <c r="H3" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I3" s="46"/>
+    </row>
+    <row r="4" spans="2:10">
       <c r="B4" s="31">
+        <v>2</v>
+      </c>
+      <c r="C4" s="50"/>
+      <c r="D4" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="H4" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I4" s="46"/>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5" s="31">
+        <v>3</v>
+      </c>
+      <c r="C5" s="50"/>
+      <c r="D5" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="H5" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I5" s="46"/>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" s="31">
+        <v>4</v>
+      </c>
+      <c r="C6" s="50"/>
+      <c r="D6" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="H6" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I6" s="46"/>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" s="31">
+        <v>5</v>
+      </c>
+      <c r="C7" s="50"/>
+      <c r="D7" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="H7" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I7" s="46"/>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" s="31">
+        <v>6</v>
+      </c>
+      <c r="C8" s="50"/>
+      <c r="D8" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="H8" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I8" s="46"/>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" s="31">
+        <v>7</v>
+      </c>
+      <c r="C9" s="50"/>
+      <c r="D9" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="H9" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I9" s="46"/>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" s="31">
+        <v>8</v>
+      </c>
+      <c r="C10" s="50"/>
+      <c r="D10" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="H10" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I10" s="46"/>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11" s="31">
+        <v>9</v>
+      </c>
+      <c r="C11" s="50"/>
+      <c r="D11" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="H11" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I11" s="46"/>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12" s="31">
+        <v>10</v>
+      </c>
+      <c r="C12" s="50"/>
+      <c r="D12" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="H12" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I12" s="46"/>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" s="31">
+        <v>11</v>
+      </c>
+      <c r="C13" s="50"/>
+      <c r="D13" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="G4" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H4" s="47"/>
-      <c r="I4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9">
-      <c r="B5" s="31">
-        <v>45</v>
-      </c>
-      <c r="C5" s="52" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>242</v>
-      </c>
-      <c r="G5" s="36" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9">
-      <c r="B6" s="31">
-        <v>2</v>
-      </c>
-      <c r="C6" s="53" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="G6" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H6" s="47"/>
-    </row>
-    <row r="7" spans="2:9">
-      <c r="B7" s="31">
+      <c r="E13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="52" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="G7" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H7" s="47"/>
-    </row>
-    <row r="8" spans="2:9">
-      <c r="B8" s="31">
-        <v>46</v>
-      </c>
-      <c r="C8" s="52" t="s">
-        <v>96</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="G8" s="36" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9">
-      <c r="B9" s="31">
-        <v>3</v>
-      </c>
-      <c r="C9" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="G9" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H9" s="47"/>
-    </row>
-    <row r="10" spans="2:9">
-      <c r="B10" s="31">
+      <c r="F13" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="H13" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I13" s="46"/>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" s="31">
+        <v>12</v>
+      </c>
+      <c r="C14" s="50"/>
+      <c r="D14" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="G10" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H10" s="47"/>
-    </row>
-    <row r="11" spans="2:9">
-      <c r="B11" s="31">
-        <v>47</v>
-      </c>
-      <c r="C11" s="38" t="s">
-        <v>97</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="G11" s="36" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9">
-      <c r="B12" s="31">
-        <v>4</v>
-      </c>
-      <c r="C12" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="G12" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H12" s="47"/>
-    </row>
-    <row r="13" spans="2:9">
-      <c r="B13" s="31">
+      <c r="E14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="G13" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H13" s="47"/>
-    </row>
-    <row r="14" spans="2:9">
-      <c r="B14" s="31">
-        <v>48</v>
-      </c>
-      <c r="C14" s="38" t="s">
-        <v>98</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="G14" s="36" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9">
+      <c r="F14" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="H14" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I14" s="46"/>
+    </row>
+    <row r="15" spans="2:10">
       <c r="B15" s="31">
-        <v>5</v>
-      </c>
-      <c r="C15" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="G15" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H15" s="47"/>
-    </row>
-    <row r="16" spans="2:9">
+        <v>13</v>
+      </c>
+      <c r="C15" s="50"/>
+      <c r="D15" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="H15" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I15" s="46"/>
+    </row>
+    <row r="16" spans="2:10">
       <c r="B16" s="31">
-        <v>27</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="G16" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H16" s="47"/>
+        <v>14</v>
+      </c>
+      <c r="C16" s="50"/>
+      <c r="D16" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="H16" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I16" s="46"/>
     </row>
     <row r="17" spans="2:9">
       <c r="B17" s="31">
-        <v>49</v>
-      </c>
-      <c r="C17" s="38" t="s">
-        <v>99</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="G17" s="36" t="s">
-        <v>257</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C17" s="50"/>
+      <c r="D17" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="H17" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I17" s="46"/>
     </row>
     <row r="18" spans="2:9">
       <c r="B18" s="31">
-        <v>6</v>
-      </c>
-      <c r="C18" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="G18" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H18" s="47"/>
+        <v>16</v>
+      </c>
+      <c r="C18" s="50"/>
+      <c r="D18" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="H18" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I18" s="46"/>
     </row>
     <row r="19" spans="2:9">
       <c r="B19" s="31">
-        <v>28</v>
-      </c>
-      <c r="C19" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="G19" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H19" s="47"/>
+        <v>17</v>
+      </c>
+      <c r="C19" s="50"/>
+      <c r="D19" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="H19" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I19" s="46"/>
     </row>
     <row r="20" spans="2:9">
       <c r="B20" s="31">
-        <v>50</v>
-      </c>
-      <c r="C20" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="D20" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="G20" s="36" t="s">
-        <v>257</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C20" s="50"/>
+      <c r="D20" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="H20" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I20" s="46"/>
     </row>
     <row r="21" spans="2:9">
       <c r="B21" s="31">
-        <v>7</v>
-      </c>
-      <c r="C21" s="53" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>286</v>
-      </c>
-      <c r="G21" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H21" s="47"/>
+        <v>19</v>
+      </c>
+      <c r="C21" s="50"/>
+      <c r="D21" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="H21" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I21" s="46"/>
     </row>
     <row r="22" spans="2:9">
       <c r="B22" s="31">
-        <v>8</v>
-      </c>
-      <c r="C22" s="53" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="G22" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H22" s="47"/>
+        <v>20</v>
+      </c>
+      <c r="C22" s="50"/>
+      <c r="D22" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="H22" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I22" s="46"/>
     </row>
     <row r="23" spans="2:9">
       <c r="B23" s="31">
-        <v>29</v>
-      </c>
-      <c r="C23" s="52" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="G23" s="36" t="s">
-        <v>257</v>
-      </c>
-      <c r="H23" s="48"/>
+        <v>21</v>
+      </c>
+      <c r="C23" s="50"/>
+      <c r="D23" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="H23" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I23" s="46"/>
     </row>
     <row r="24" spans="2:9">
       <c r="B24" s="31">
-        <v>51</v>
-      </c>
-      <c r="C24" s="52" t="s">
-        <v>101</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="G24" s="36" t="s">
-        <v>257</v>
-      </c>
-      <c r="I24" s="41"/>
+        <v>22</v>
+      </c>
+      <c r="C24" s="50"/>
+      <c r="D24" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="H24" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I24" s="46"/>
     </row>
     <row r="25" spans="2:9">
       <c r="B25" s="31">
-        <v>9</v>
-      </c>
-      <c r="C25" s="53" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="G25" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H25" s="47"/>
+        <v>23</v>
+      </c>
+      <c r="C25" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="H25" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I25" s="46"/>
     </row>
     <row r="26" spans="2:9">
       <c r="B26" s="31">
-        <v>30</v>
-      </c>
-      <c r="C26" s="52" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E26" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="G26" s="36" t="s">
-        <v>257</v>
-      </c>
-      <c r="H26" s="48"/>
+        <v>24</v>
+      </c>
+      <c r="C26" s="50"/>
+      <c r="D26" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="H26" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I26" s="46"/>
     </row>
     <row r="27" spans="2:9">
       <c r="B27" s="31">
-        <v>52</v>
-      </c>
-      <c r="C27" s="52" t="s">
-        <v>102</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="G27" s="36" t="s">
-        <v>257</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C27" s="50"/>
+      <c r="D27" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="H27" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I27" s="46"/>
     </row>
     <row r="28" spans="2:9">
       <c r="B28" s="31">
-        <v>10</v>
-      </c>
-      <c r="C28" s="53" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="G28" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H28" s="47"/>
+        <v>26</v>
+      </c>
+      <c r="C28" s="50"/>
+      <c r="D28" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="H28" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I28" s="46"/>
     </row>
     <row r="29" spans="2:9">
       <c r="B29" s="31">
-        <v>31</v>
-      </c>
-      <c r="C29" s="52" t="s">
-        <v>66</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="G29" s="36" t="s">
-        <v>257</v>
-      </c>
-      <c r="H29" s="48"/>
+        <v>27</v>
+      </c>
+      <c r="C29" s="50"/>
+      <c r="D29" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="H29" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I29" s="46"/>
     </row>
     <row r="30" spans="2:9">
       <c r="B30" s="31">
-        <v>53</v>
-      </c>
-      <c r="C30" s="52" t="s">
-        <v>103</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="G30" s="36" t="s">
-        <v>257</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C30" s="50"/>
+      <c r="D30" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="H30" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I30" s="46"/>
     </row>
     <row r="31" spans="2:9">
       <c r="B31" s="31">
-        <v>11</v>
-      </c>
-      <c r="C31" s="53" t="s">
-        <v>23</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E31" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="G31" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H31" s="47"/>
+        <v>29</v>
+      </c>
+      <c r="C31" s="50"/>
+      <c r="D31" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="H31" s="49" t="s">
+        <v>257</v>
+      </c>
+      <c r="I31" s="47"/>
     </row>
     <row r="32" spans="2:9">
       <c r="B32" s="31">
+        <v>30</v>
+      </c>
+      <c r="C32" s="50"/>
+      <c r="D32" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F32" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="H32" s="49" t="s">
+        <v>257</v>
+      </c>
+      <c r="I32" s="47"/>
+    </row>
+    <row r="33" spans="2:9">
+      <c r="B33" s="31">
+        <v>31</v>
+      </c>
+      <c r="C33" s="50"/>
+      <c r="D33" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="H33" s="49" t="s">
+        <v>257</v>
+      </c>
+      <c r="I33" s="47"/>
+    </row>
+    <row r="34" spans="2:9">
+      <c r="B34" s="31">
         <v>32</v>
       </c>
-      <c r="C32" s="52" t="s">
+      <c r="C34" s="50"/>
+      <c r="D34" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="D32" s="28" t="s">
+      <c r="E34" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E32" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F32" s="7" t="s">
+      <c r="F34" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G34" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="G32" s="36" t="s">
-        <v>257</v>
-      </c>
-      <c r="H32" s="48"/>
-    </row>
-    <row r="33" spans="2:8">
-      <c r="B33" s="31">
-        <v>54</v>
-      </c>
-      <c r="C33" s="52" t="s">
-        <v>104</v>
-      </c>
-      <c r="D33" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F33" s="28" t="s">
-        <v>253</v>
-      </c>
-      <c r="G33" s="36" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8">
-      <c r="B34" s="31">
-        <v>12</v>
-      </c>
-      <c r="C34" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="G34" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H34" s="47"/>
-    </row>
-    <row r="35" spans="2:8">
+      <c r="H34" s="49" t="s">
+        <v>257</v>
+      </c>
+      <c r="I34" s="47"/>
+    </row>
+    <row r="35" spans="2:9">
       <c r="B35" s="31">
         <v>33</v>
       </c>
-      <c r="C35" s="22" t="s">
+      <c r="C35" s="50"/>
+      <c r="D35" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="E35" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E35" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F35" s="7" t="s">
+      <c r="F35" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G35" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="G35" s="36" t="s">
-        <v>257</v>
-      </c>
-      <c r="H35" s="48"/>
-    </row>
-    <row r="36" spans="2:8">
+      <c r="H35" s="49" t="s">
+        <v>257</v>
+      </c>
+      <c r="I35" s="47"/>
+    </row>
+    <row r="36" spans="2:9">
       <c r="B36" s="31">
+        <v>34</v>
+      </c>
+      <c r="C36" s="50"/>
+      <c r="D36" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="H36" s="49" t="s">
+        <v>257</v>
+      </c>
+      <c r="I36" s="47"/>
+    </row>
+    <row r="37" spans="2:9">
+      <c r="B37" s="31">
+        <v>35</v>
+      </c>
+      <c r="C37" s="50"/>
+      <c r="D37" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="E37" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="H37" s="49" t="s">
+        <v>257</v>
+      </c>
+      <c r="I37" s="47"/>
+    </row>
+    <row r="38" spans="2:9">
+      <c r="B38" s="31">
+        <v>36</v>
+      </c>
+      <c r="C38" s="50"/>
+      <c r="D38" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="H38" s="49" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9">
+      <c r="B39" s="31">
+        <v>37</v>
+      </c>
+      <c r="C39" s="50"/>
+      <c r="D39" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="H39" s="49" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9">
+      <c r="B40" s="31">
+        <v>38</v>
+      </c>
+      <c r="C40" s="50"/>
+      <c r="D40" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="H40" s="49" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9">
+      <c r="B41" s="31">
+        <v>39</v>
+      </c>
+      <c r="C41" s="50"/>
+      <c r="D41" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F41" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="H41" s="49" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9">
+      <c r="B42" s="31">
+        <v>40</v>
+      </c>
+      <c r="C42" s="50"/>
+      <c r="D42" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G42" s="41" t="s">
+        <v>306</v>
+      </c>
+      <c r="H42" s="49" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9">
+      <c r="B43" s="31">
+        <v>41</v>
+      </c>
+      <c r="C43" s="50"/>
+      <c r="D43" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F43" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="H43" s="49" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9">
+      <c r="B44" s="31">
+        <v>42</v>
+      </c>
+      <c r="C44" s="50"/>
+      <c r="D44" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F44" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="H44" s="49" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9">
+      <c r="B45" s="31">
+        <v>43</v>
+      </c>
+      <c r="C45" s="50"/>
+      <c r="D45" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F45" s="36" t="s">
+        <v>194</v>
+      </c>
+      <c r="G45" s="45" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9">
+      <c r="B46" s="31">
+        <v>44</v>
+      </c>
+      <c r="C46" s="50"/>
+      <c r="D46" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="H46" s="49" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" ht="14.5" customHeight="1">
+      <c r="B47" s="31">
+        <v>45</v>
+      </c>
+      <c r="C47" s="50" t="s">
+        <v>118</v>
+      </c>
+      <c r="D47" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F47" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G47" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="H47" s="49" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9">
+      <c r="B48" s="31">
+        <v>46</v>
+      </c>
+      <c r="C48" s="50"/>
+      <c r="D48" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F48" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="H48" s="49" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11">
+      <c r="B49" s="31">
+        <v>47</v>
+      </c>
+      <c r="C49" s="50"/>
+      <c r="D49" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F49" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="H49" s="49" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11">
+      <c r="B50" s="31">
+        <v>48</v>
+      </c>
+      <c r="C50" s="50"/>
+      <c r="D50" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F50" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="H50" s="49" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11">
+      <c r="B51" s="31">
+        <v>49</v>
+      </c>
+      <c r="C51" s="50"/>
+      <c r="D51" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F51" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="H51" s="49" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11">
+      <c r="B52" s="31">
+        <v>50</v>
+      </c>
+      <c r="C52" s="50"/>
+      <c r="D52" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="E52" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F52" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="H52" s="49" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11">
+      <c r="B53" s="31">
+        <v>51</v>
+      </c>
+      <c r="C53" s="50"/>
+      <c r="D53" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F53" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="H53" s="49" t="s">
+        <v>257</v>
+      </c>
+      <c r="J53" s="40"/>
+      <c r="K53" s="39"/>
+    </row>
+    <row r="54" spans="2:11">
+      <c r="B54" s="31">
+        <v>52</v>
+      </c>
+      <c r="C54" s="50"/>
+      <c r="D54" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F54" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="H54" s="49" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11">
+      <c r="B55" s="31">
+        <v>53</v>
+      </c>
+      <c r="C55" s="50"/>
+      <c r="D55" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F55" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="H55" s="49" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11">
+      <c r="B56" s="31">
+        <v>54</v>
+      </c>
+      <c r="C56" s="50"/>
+      <c r="D56" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="E56" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="F56" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G56" s="28" t="s">
+        <v>253</v>
+      </c>
+      <c r="H56" s="49" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11">
+      <c r="B57" s="31">
         <v>55</v>
       </c>
-      <c r="C36" s="23" t="s">
+      <c r="C57" s="50"/>
+      <c r="D57" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E57" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E36" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F36" s="7" t="s">
+      <c r="F57" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G57" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="G36" s="36" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8">
-      <c r="B37" s="31">
-        <v>13</v>
-      </c>
-      <c r="C37" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="G37" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H37" s="47"/>
-    </row>
-    <row r="38" spans="2:8">
-      <c r="B38" s="31">
-        <v>34</v>
-      </c>
-      <c r="C38" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E38" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="G38" s="36" t="s">
-        <v>257</v>
-      </c>
-      <c r="H38" s="48"/>
-    </row>
-    <row r="39" spans="2:8">
-      <c r="B39" s="31">
+      <c r="H57" s="49" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="58" spans="2:11">
+      <c r="B58" s="31">
         <v>56</v>
       </c>
-      <c r="C39" s="27" t="s">
+      <c r="C58" s="50"/>
+      <c r="D58" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="D39" s="29" t="s">
+      <c r="E58" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="E39" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F39" s="7" t="s">
+      <c r="F58" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G58" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="G39" s="36" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8">
-      <c r="B40" s="31">
-        <v>14</v>
-      </c>
-      <c r="C40" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D40" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="E40" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="G40" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H40" s="47"/>
-    </row>
-    <row r="41" spans="2:8">
-      <c r="B41" s="31">
-        <v>35</v>
-      </c>
-      <c r="C41" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="D41" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="E41" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="G41" s="36" t="s">
-        <v>257</v>
-      </c>
-      <c r="H41" s="48"/>
-    </row>
-    <row r="42" spans="2:8">
-      <c r="B42" s="31">
+      <c r="H58" s="49" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11">
+      <c r="B59" s="31">
         <v>57</v>
       </c>
-      <c r="C42" s="23" t="s">
+      <c r="C59" s="50"/>
+      <c r="D59" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="D42" s="29" t="s">
+      <c r="E59" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="E42" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F42" s="7" t="s">
+      <c r="F59" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G59" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="G42" s="36" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8">
-      <c r="B43" s="31">
-        <v>15</v>
-      </c>
-      <c r="C43" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E43" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="G43" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H43" s="47"/>
-    </row>
-    <row r="44" spans="2:8">
-      <c r="B44" s="31">
-        <v>36</v>
-      </c>
-      <c r="C44" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E44" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="G44" s="36" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8">
-      <c r="B45" s="31">
+      <c r="H59" s="49" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11">
+      <c r="B60" s="31">
         <v>58</v>
       </c>
-      <c r="C45" s="39" t="s">
+      <c r="C60" s="50"/>
+      <c r="D60" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="E60" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E45" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F45" s="7" t="s">
+      <c r="F60" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G60" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="G45" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H45" s="47"/>
-    </row>
-    <row r="46" spans="2:8">
-      <c r="B46" s="31">
-        <v>16</v>
-      </c>
-      <c r="C46" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E46" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>292</v>
-      </c>
-      <c r="G46" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H46" s="47"/>
-    </row>
-    <row r="47" spans="2:8" ht="14.5" customHeight="1">
-      <c r="B47" s="31">
-        <v>37</v>
-      </c>
-      <c r="C47" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E47" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="G47" s="36" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8">
-      <c r="B48" s="31">
+      <c r="H60" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I60" s="46"/>
+    </row>
+    <row r="61" spans="2:11">
+      <c r="B61" s="31">
         <v>59</v>
       </c>
-      <c r="C48" s="23" t="s">
+      <c r="C61" s="50"/>
+      <c r="D61" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="E61" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E48" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F48" s="7" t="s">
+      <c r="F61" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G61" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="G48" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H48" s="47"/>
-    </row>
-    <row r="49" spans="2:10">
-      <c r="B49" s="31">
-        <v>17</v>
-      </c>
-      <c r="C49" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E49" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="G49" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H49" s="47"/>
-    </row>
-    <row r="50" spans="2:10">
-      <c r="B50" s="31">
-        <v>38</v>
-      </c>
-      <c r="C50" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E50" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="G50" s="36" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="51" spans="2:10">
-      <c r="B51" s="31">
+      <c r="H61" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I61" s="46"/>
+    </row>
+    <row r="62" spans="2:11">
+      <c r="B62" s="31">
         <v>60</v>
       </c>
-      <c r="C51" s="23" t="s">
+      <c r="C62" s="50"/>
+      <c r="D62" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="E62" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E51" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F51" s="7" t="s">
+      <c r="F62" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G62" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="G51" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H51" s="47"/>
-    </row>
-    <row r="52" spans="2:10">
-      <c r="B52" s="31">
-        <v>18</v>
-      </c>
-      <c r="C52" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E52" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="G52" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H52" s="47"/>
-    </row>
-    <row r="53" spans="2:10">
-      <c r="B53" s="31">
-        <v>39</v>
-      </c>
-      <c r="C53" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="E53" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F53" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G53" s="36" t="s">
-        <v>257</v>
-      </c>
-      <c r="J53" s="40"/>
-    </row>
-    <row r="54" spans="2:10">
-      <c r="B54" s="31">
+      <c r="H62" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I62" s="46"/>
+    </row>
+    <row r="63" spans="2:11">
+      <c r="B63" s="31">
         <v>61</v>
       </c>
-      <c r="C54" s="25" t="s">
+      <c r="C63" s="50"/>
+      <c r="D63" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="E63" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E54" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F54" s="7" t="s">
+      <c r="F63" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G63" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="G54" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H54" s="47"/>
-    </row>
-    <row r="55" spans="2:10">
-      <c r="B55" s="31">
-        <v>19</v>
-      </c>
-      <c r="C55" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E55" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>305</v>
-      </c>
-      <c r="G55" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H55" s="47"/>
-    </row>
-    <row r="56" spans="2:10">
-      <c r="B56" s="31">
-        <v>40</v>
-      </c>
-      <c r="C56" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="D56" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E56" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F56" s="42" t="s">
-        <v>306</v>
-      </c>
-      <c r="G56" s="36" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="57" spans="2:10">
-      <c r="B57" s="31">
+      <c r="H63" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I63" s="46"/>
+    </row>
+    <row r="64" spans="2:11">
+      <c r="B64" s="31">
         <v>62</v>
       </c>
-      <c r="C57" s="25" t="s">
+      <c r="C64" s="50"/>
+      <c r="D64" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="E64" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E57" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F57" s="42" t="s">
+      <c r="F64" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G64" s="41" t="s">
         <v>307</v>
       </c>
-      <c r="G57" s="36" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="58" spans="2:10">
-      <c r="B58" s="31">
-        <v>20</v>
-      </c>
-      <c r="C58" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E58" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F58" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="G58" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H58" s="47"/>
-    </row>
-    <row r="59" spans="2:10">
-      <c r="B59" s="31">
-        <v>41</v>
-      </c>
-      <c r="C59" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E59" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F59" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="G59" s="36" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="60" spans="2:10">
-      <c r="B60" s="31">
-        <v>63</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="E60" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="G60" s="36" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="61" spans="2:10">
-      <c r="B61" s="31">
-        <v>21</v>
-      </c>
-      <c r="C61" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="D61" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E61" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F61" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="G61" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H61" s="47"/>
-    </row>
-    <row r="62" spans="2:10">
-      <c r="B62" s="31">
-        <v>42</v>
-      </c>
-      <c r="C62" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E62" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F62" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="G62" s="36" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="63" spans="2:10">
-      <c r="B63" s="31">
-        <v>64</v>
-      </c>
-      <c r="C63" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E63" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F63" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="G63" s="36" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="64" spans="2:10">
-      <c r="B64" s="37">
-        <v>43</v>
-      </c>
-      <c r="C64" s="38" t="s">
-        <v>90</v>
-      </c>
-      <c r="D64" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="E64" s="37" t="s">
-        <v>194</v>
-      </c>
-      <c r="F64" s="46" t="s">
-        <v>314</v>
+      <c r="H64" s="49" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="65" spans="2:8">
       <c r="B65" s="31">
-        <v>22</v>
-      </c>
-      <c r="C65" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D65" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E65" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F65" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="G65" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H65" s="47"/>
+        <v>63</v>
+      </c>
+      <c r="C65" s="50"/>
+      <c r="D65" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F65" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G65" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="H65" s="49" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="66" spans="2:8">
       <c r="B66" s="31">
-        <v>44</v>
-      </c>
-      <c r="C66" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E66" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F66" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="G66" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C66" s="50"/>
+      <c r="D66" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F66" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G66" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="H66" s="49" t="s">
         <v>257</v>
       </c>
     </row>
@@ -3494,26 +3556,29 @@
       <c r="B67" s="31">
         <v>65</v>
       </c>
-      <c r="C67" s="25" t="s">
+      <c r="C67" s="50"/>
+      <c r="D67" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="E67" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="E67" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F67" s="7" t="s">
+      <c r="F67" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G67" s="7" t="s">
         <v>317</v>
       </c>
-      <c r="G67" s="36" t="s">
+      <c r="H67" s="49" t="s">
         <v>257</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:I67">
-    <sortCondition ref="C1:C67"/>
-  </sortState>
+  <mergeCells count="3">
+    <mergeCell ref="C3:C24"/>
+    <mergeCell ref="C25:C46"/>
+    <mergeCell ref="C47:C67"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3572,7 +3637,7 @@
       <c r="B3" s="11">
         <v>1</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="50" t="s">
         <v>48</v>
       </c>
       <c r="D3" s="24" t="s">
@@ -3590,13 +3655,13 @@
       <c r="H3" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I3" s="47"/>
+      <c r="I3" s="46"/>
     </row>
     <row r="4" spans="2:10">
       <c r="B4" s="11">
         <v>2</v>
       </c>
-      <c r="C4" s="49"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="19" t="s">
         <v>5</v>
       </c>
@@ -3612,13 +3677,13 @@
       <c r="H4" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I4" s="47"/>
+      <c r="I4" s="46"/>
     </row>
     <row r="5" spans="2:10">
       <c r="B5" s="11">
         <v>3</v>
       </c>
-      <c r="C5" s="49"/>
+      <c r="C5" s="50"/>
       <c r="D5" s="9" t="s">
         <v>7</v>
       </c>
@@ -3634,13 +3699,13 @@
       <c r="H5" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I5" s="47"/>
+      <c r="I5" s="46"/>
     </row>
     <row r="6" spans="2:10">
       <c r="B6" s="11">
         <v>4</v>
       </c>
-      <c r="C6" s="49"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="21" t="s">
         <v>9</v>
       </c>
@@ -3656,13 +3721,13 @@
       <c r="H6" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I6" s="47"/>
+      <c r="I6" s="46"/>
     </row>
     <row r="7" spans="2:10">
       <c r="B7" s="11">
         <v>5</v>
       </c>
-      <c r="C7" s="49"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="24" t="s">
         <v>11</v>
       </c>
@@ -3678,13 +3743,13 @@
       <c r="H7" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I7" s="47"/>
+      <c r="I7" s="46"/>
     </row>
     <row r="8" spans="2:10">
       <c r="B8" s="11">
         <v>6</v>
       </c>
-      <c r="C8" s="49"/>
+      <c r="C8" s="50"/>
       <c r="D8" s="9" t="s">
         <v>13</v>
       </c>
@@ -3700,13 +3765,13 @@
       <c r="H8" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I8" s="47"/>
+      <c r="I8" s="46"/>
     </row>
     <row r="9" spans="2:10">
       <c r="B9" s="11">
         <v>7</v>
       </c>
-      <c r="C9" s="49"/>
+      <c r="C9" s="50"/>
       <c r="D9" s="16" t="s">
         <v>15</v>
       </c>
@@ -3722,13 +3787,13 @@
       <c r="H9" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I9" s="47"/>
+      <c r="I9" s="46"/>
     </row>
     <row r="10" spans="2:10">
       <c r="B10" s="11">
         <v>8</v>
       </c>
-      <c r="C10" s="49"/>
+      <c r="C10" s="50"/>
       <c r="D10" s="17" t="s">
         <v>17</v>
       </c>
@@ -3744,13 +3809,13 @@
       <c r="H10" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I10" s="47"/>
+      <c r="I10" s="46"/>
     </row>
     <row r="11" spans="2:10">
       <c r="B11" s="11">
         <v>9</v>
       </c>
-      <c r="C11" s="49"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="17" t="s">
         <v>19</v>
       </c>
@@ -3766,13 +3831,13 @@
       <c r="H11" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I11" s="47"/>
+      <c r="I11" s="46"/>
     </row>
     <row r="12" spans="2:10">
       <c r="B12" s="11">
         <v>10</v>
       </c>
-      <c r="C12" s="49"/>
+      <c r="C12" s="50"/>
       <c r="D12" s="19" t="s">
         <v>21</v>
       </c>
@@ -3788,13 +3853,13 @@
       <c r="H12" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I12" s="47"/>
+      <c r="I12" s="46"/>
     </row>
     <row r="13" spans="2:10">
       <c r="B13" s="11">
         <v>11</v>
       </c>
-      <c r="C13" s="49"/>
+      <c r="C13" s="50"/>
       <c r="D13" s="19" t="s">
         <v>23</v>
       </c>
@@ -3810,13 +3875,13 @@
       <c r="H13" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I13" s="47"/>
+      <c r="I13" s="46"/>
     </row>
     <row r="14" spans="2:10">
       <c r="B14" s="11">
         <v>12</v>
       </c>
-      <c r="C14" s="49"/>
+      <c r="C14" s="50"/>
       <c r="D14" s="19" t="s">
         <v>25</v>
       </c>
@@ -3832,13 +3897,13 @@
       <c r="H14" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I14" s="47"/>
+      <c r="I14" s="46"/>
     </row>
     <row r="15" spans="2:10">
       <c r="B15" s="11">
         <v>13</v>
       </c>
-      <c r="C15" s="49"/>
+      <c r="C15" s="50"/>
       <c r="D15" s="16" t="s">
         <v>27</v>
       </c>
@@ -3854,13 +3919,13 @@
       <c r="H15" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I15" s="47"/>
+      <c r="I15" s="46"/>
     </row>
     <row r="16" spans="2:10">
       <c r="B16" s="11">
         <v>14</v>
       </c>
-      <c r="C16" s="49"/>
+      <c r="C16" s="50"/>
       <c r="D16" s="24" t="s">
         <v>29</v>
       </c>
@@ -3876,13 +3941,13 @@
       <c r="H16" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I16" s="47"/>
+      <c r="I16" s="46"/>
     </row>
     <row r="17" spans="2:9">
       <c r="B17" s="11">
         <v>15</v>
       </c>
-      <c r="C17" s="49"/>
+      <c r="C17" s="50"/>
       <c r="D17" s="31" t="s">
         <v>31</v>
       </c>
@@ -3898,13 +3963,13 @@
       <c r="H17" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I17" s="47"/>
+      <c r="I17" s="46"/>
     </row>
     <row r="18" spans="2:9">
       <c r="B18" s="11">
         <v>16</v>
       </c>
-      <c r="C18" s="49"/>
+      <c r="C18" s="50"/>
       <c r="D18" s="24" t="s">
         <v>33</v>
       </c>
@@ -3920,13 +3985,13 @@
       <c r="H18" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I18" s="47"/>
+      <c r="I18" s="46"/>
     </row>
     <row r="19" spans="2:9">
       <c r="B19" s="11">
         <v>17</v>
       </c>
-      <c r="C19" s="49"/>
+      <c r="C19" s="50"/>
       <c r="D19" s="24" t="s">
         <v>35</v>
       </c>
@@ -3942,13 +4007,13 @@
       <c r="H19" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I19" s="47"/>
+      <c r="I19" s="46"/>
     </row>
     <row r="20" spans="2:9">
       <c r="B20" s="11">
         <v>18</v>
       </c>
-      <c r="C20" s="49"/>
+      <c r="C20" s="50"/>
       <c r="D20" s="31" t="s">
         <v>37</v>
       </c>
@@ -3964,13 +4029,13 @@
       <c r="H20" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I20" s="47"/>
+      <c r="I20" s="46"/>
     </row>
     <row r="21" spans="2:9">
       <c r="B21" s="11">
         <v>19</v>
       </c>
-      <c r="C21" s="49"/>
+      <c r="C21" s="50"/>
       <c r="D21" s="24" t="s">
         <v>39</v>
       </c>
@@ -3986,13 +4051,13 @@
       <c r="H21" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I21" s="47"/>
+      <c r="I21" s="46"/>
     </row>
     <row r="22" spans="2:9">
       <c r="B22" s="11">
         <v>20</v>
       </c>
-      <c r="C22" s="49"/>
+      <c r="C22" s="50"/>
       <c r="D22" s="31" t="s">
         <v>41</v>
       </c>
@@ -4008,13 +4073,13 @@
       <c r="H22" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I22" s="47"/>
+      <c r="I22" s="46"/>
     </row>
     <row r="23" spans="2:9">
       <c r="B23" s="11">
         <v>21</v>
       </c>
-      <c r="C23" s="49"/>
+      <c r="C23" s="50"/>
       <c r="D23" s="24" t="s">
         <v>43</v>
       </c>
@@ -4030,13 +4095,13 @@
       <c r="H23" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I23" s="47"/>
+      <c r="I23" s="46"/>
     </row>
     <row r="24" spans="2:9">
       <c r="B24" s="11">
         <v>22</v>
       </c>
-      <c r="C24" s="49"/>
+      <c r="C24" s="50"/>
       <c r="D24" s="31" t="s">
         <v>45</v>
       </c>
@@ -4052,13 +4117,13 @@
       <c r="H24" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I24" s="47"/>
+      <c r="I24" s="46"/>
     </row>
     <row r="25" spans="2:9">
       <c r="B25" s="11">
         <v>23</v>
       </c>
-      <c r="C25" s="49" t="s">
+      <c r="C25" s="50" t="s">
         <v>94</v>
       </c>
       <c r="D25" s="23" t="s">
@@ -4076,13 +4141,13 @@
       <c r="H25" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I25" s="47"/>
+      <c r="I25" s="46"/>
     </row>
     <row r="26" spans="2:9">
       <c r="B26" s="11">
         <v>24</v>
       </c>
-      <c r="C26" s="49"/>
+      <c r="C26" s="50"/>
       <c r="D26" s="18" t="s">
         <v>52</v>
       </c>
@@ -4098,13 +4163,13 @@
       <c r="H26" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I26" s="47"/>
+      <c r="I26" s="46"/>
     </row>
     <row r="27" spans="2:9">
       <c r="B27" s="11">
         <v>25</v>
       </c>
-      <c r="C27" s="49"/>
+      <c r="C27" s="50"/>
       <c r="D27" s="6" t="s">
         <v>54</v>
       </c>
@@ -4120,13 +4185,13 @@
       <c r="H27" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I27" s="47"/>
+      <c r="I27" s="46"/>
     </row>
     <row r="28" spans="2:9">
       <c r="B28" s="11">
         <v>26</v>
       </c>
-      <c r="C28" s="49"/>
+      <c r="C28" s="50"/>
       <c r="D28" s="25" t="s">
         <v>56</v>
       </c>
@@ -4142,13 +4207,13 @@
       <c r="H28" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I28" s="47"/>
+      <c r="I28" s="46"/>
     </row>
     <row r="29" spans="2:9">
       <c r="B29" s="11">
         <v>27</v>
       </c>
-      <c r="C29" s="49"/>
+      <c r="C29" s="50"/>
       <c r="D29" s="23" t="s">
         <v>58</v>
       </c>
@@ -4164,13 +4229,13 @@
       <c r="H29" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I29" s="47"/>
+      <c r="I29" s="46"/>
     </row>
     <row r="30" spans="2:9">
       <c r="B30" s="11">
         <v>28</v>
       </c>
-      <c r="C30" s="49"/>
+      <c r="C30" s="50"/>
       <c r="D30" s="25" t="s">
         <v>60</v>
       </c>
@@ -4186,13 +4251,13 @@
       <c r="H30" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I30" s="47"/>
+      <c r="I30" s="46"/>
     </row>
     <row r="31" spans="2:9">
       <c r="B31" s="11">
         <v>29</v>
       </c>
-      <c r="C31" s="49"/>
+      <c r="C31" s="50"/>
       <c r="D31" s="18" t="s">
         <v>62</v>
       </c>
@@ -4208,13 +4273,13 @@
       <c r="H31" s="33" t="s">
         <v>257</v>
       </c>
-      <c r="I31" s="48"/>
+      <c r="I31" s="47"/>
     </row>
     <row r="32" spans="2:9">
       <c r="B32" s="11">
         <v>30</v>
       </c>
-      <c r="C32" s="49"/>
+      <c r="C32" s="50"/>
       <c r="D32" s="27" t="s">
         <v>64</v>
       </c>
@@ -4230,13 +4295,13 @@
       <c r="H32" s="33" t="s">
         <v>257</v>
       </c>
-      <c r="I32" s="48"/>
+      <c r="I32" s="47"/>
     </row>
     <row r="33" spans="2:9">
       <c r="B33" s="11">
         <v>31</v>
       </c>
-      <c r="C33" s="49"/>
+      <c r="C33" s="50"/>
       <c r="D33" s="22" t="s">
         <v>66</v>
       </c>
@@ -4252,13 +4317,13 @@
       <c r="H33" s="33" t="s">
         <v>257</v>
       </c>
-      <c r="I33" s="48"/>
+      <c r="I33" s="47"/>
     </row>
     <row r="34" spans="2:9">
       <c r="B34" s="11">
         <v>32</v>
       </c>
-      <c r="C34" s="49"/>
+      <c r="C34" s="50"/>
       <c r="D34" s="27" t="s">
         <v>68</v>
       </c>
@@ -4274,13 +4339,13 @@
       <c r="H34" s="33" t="s">
         <v>257</v>
       </c>
-      <c r="I34" s="48"/>
+      <c r="I34" s="47"/>
     </row>
     <row r="35" spans="2:9">
       <c r="B35" s="11">
         <v>33</v>
       </c>
-      <c r="C35" s="49"/>
+      <c r="C35" s="50"/>
       <c r="D35" s="22" t="s">
         <v>70</v>
       </c>
@@ -4296,13 +4361,13 @@
       <c r="H35" s="33" t="s">
         <v>257</v>
       </c>
-      <c r="I35" s="48"/>
+      <c r="I35" s="47"/>
     </row>
     <row r="36" spans="2:9">
       <c r="B36" s="11">
         <v>34</v>
       </c>
-      <c r="C36" s="49"/>
+      <c r="C36" s="50"/>
       <c r="D36" s="27" t="s">
         <v>72</v>
       </c>
@@ -4318,13 +4383,13 @@
       <c r="H36" s="33" t="s">
         <v>257</v>
       </c>
-      <c r="I36" s="48"/>
+      <c r="I36" s="47"/>
     </row>
     <row r="37" spans="2:9">
       <c r="B37" s="11">
         <v>35</v>
       </c>
-      <c r="C37" s="49"/>
+      <c r="C37" s="50"/>
       <c r="D37" s="23" t="s">
         <v>74</v>
       </c>
@@ -4340,13 +4405,13 @@
       <c r="H37" s="33" t="s">
         <v>257</v>
       </c>
-      <c r="I37" s="48"/>
+      <c r="I37" s="47"/>
     </row>
     <row r="38" spans="2:9">
       <c r="B38" s="11">
         <v>36</v>
       </c>
-      <c r="C38" s="49"/>
+      <c r="C38" s="50"/>
       <c r="D38" s="25" t="s">
         <v>76</v>
       </c>
@@ -4367,7 +4432,7 @@
       <c r="B39" s="11">
         <v>37</v>
       </c>
-      <c r="C39" s="49"/>
+      <c r="C39" s="50"/>
       <c r="D39" s="23" t="s">
         <v>78</v>
       </c>
@@ -4388,7 +4453,7 @@
       <c r="B40" s="11">
         <v>38</v>
       </c>
-      <c r="C40" s="49"/>
+      <c r="C40" s="50"/>
       <c r="D40" s="23" t="s">
         <v>80</v>
       </c>
@@ -4409,7 +4474,7 @@
       <c r="B41" s="11">
         <v>39</v>
       </c>
-      <c r="C41" s="49"/>
+      <c r="C41" s="50"/>
       <c r="D41" s="23" t="s">
         <v>82</v>
       </c>
@@ -4430,7 +4495,7 @@
       <c r="B42" s="11">
         <v>40</v>
       </c>
-      <c r="C42" s="49"/>
+      <c r="C42" s="50"/>
       <c r="D42" s="23" t="s">
         <v>84</v>
       </c>
@@ -4440,7 +4505,7 @@
       <c r="F42" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="G42" s="42" t="s">
+      <c r="G42" s="41" t="s">
         <v>306</v>
       </c>
       <c r="H42" s="33" t="s">
@@ -4451,7 +4516,7 @@
       <c r="B43" s="11">
         <v>41</v>
       </c>
-      <c r="C43" s="49"/>
+      <c r="C43" s="50"/>
       <c r="D43" s="25" t="s">
         <v>86</v>
       </c>
@@ -4472,7 +4537,7 @@
       <c r="B44" s="11">
         <v>42</v>
       </c>
-      <c r="C44" s="49"/>
+      <c r="C44" s="50"/>
       <c r="D44" s="23" t="s">
         <v>88</v>
       </c>
@@ -4493,17 +4558,17 @@
       <c r="B45" s="11">
         <v>43</v>
       </c>
-      <c r="C45" s="49"/>
-      <c r="D45" s="38" t="s">
+      <c r="C45" s="50"/>
+      <c r="D45" s="37" t="s">
         <v>90</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="F45" s="37" t="s">
+      <c r="F45" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="G45" s="46" t="s">
+      <c r="G45" s="45" t="s">
         <v>314</v>
       </c>
     </row>
@@ -4511,7 +4576,7 @@
       <c r="B46" s="11">
         <v>44</v>
       </c>
-      <c r="C46" s="49"/>
+      <c r="C46" s="50"/>
       <c r="D46" s="25" t="s">
         <v>92</v>
       </c>
@@ -4532,7 +4597,7 @@
       <c r="B47" s="11">
         <v>45</v>
       </c>
-      <c r="C47" s="49" t="s">
+      <c r="C47" s="50" t="s">
         <v>118</v>
       </c>
       <c r="D47" s="27" t="s">
@@ -4555,7 +4620,7 @@
       <c r="B48" s="11">
         <v>46</v>
       </c>
-      <c r="C48" s="49"/>
+      <c r="C48" s="50"/>
       <c r="D48" s="18" t="s">
         <v>96</v>
       </c>
@@ -4576,7 +4641,7 @@
       <c r="B49" s="11">
         <v>47</v>
       </c>
-      <c r="C49" s="49"/>
+      <c r="C49" s="50"/>
       <c r="D49" s="25" t="s">
         <v>97</v>
       </c>
@@ -4597,7 +4662,7 @@
       <c r="B50" s="11">
         <v>48</v>
       </c>
-      <c r="C50" s="49"/>
+      <c r="C50" s="50"/>
       <c r="D50" s="6" t="s">
         <v>98</v>
       </c>
@@ -4618,7 +4683,7 @@
       <c r="B51" s="11">
         <v>49</v>
       </c>
-      <c r="C51" s="49"/>
+      <c r="C51" s="50"/>
       <c r="D51" s="23" t="s">
         <v>99</v>
       </c>
@@ -4639,7 +4704,7 @@
       <c r="B52" s="11">
         <v>50</v>
       </c>
-      <c r="C52" s="49"/>
+      <c r="C52" s="50"/>
       <c r="D52" s="25" t="s">
         <v>100</v>
       </c>
@@ -4660,7 +4725,7 @@
       <c r="B53" s="11">
         <v>51</v>
       </c>
-      <c r="C53" s="49"/>
+      <c r="C53" s="50"/>
       <c r="D53" s="18" t="s">
         <v>101</v>
       </c>
@@ -4676,14 +4741,14 @@
       <c r="H53" s="33" t="s">
         <v>257</v>
       </c>
-      <c r="J53" s="41"/>
-      <c r="K53" s="40"/>
+      <c r="J53" s="40"/>
+      <c r="K53" s="39"/>
     </row>
     <row r="54" spans="2:11">
       <c r="B54" s="11">
         <v>52</v>
       </c>
-      <c r="C54" s="49"/>
+      <c r="C54" s="50"/>
       <c r="D54" s="22" t="s">
         <v>102</v>
       </c>
@@ -4704,7 +4769,7 @@
       <c r="B55" s="11">
         <v>53</v>
       </c>
-      <c r="C55" s="49"/>
+      <c r="C55" s="50"/>
       <c r="D55" s="18" t="s">
         <v>103</v>
       </c>
@@ -4725,7 +4790,7 @@
       <c r="B56" s="11">
         <v>54</v>
       </c>
-      <c r="C56" s="49"/>
+      <c r="C56" s="50"/>
       <c r="D56" s="27" t="s">
         <v>104</v>
       </c>
@@ -4746,7 +4811,7 @@
       <c r="B57" s="11">
         <v>55</v>
       </c>
-      <c r="C57" s="49"/>
+      <c r="C57" s="50"/>
       <c r="D57" s="23" t="s">
         <v>115</v>
       </c>
@@ -4767,7 +4832,7 @@
       <c r="B58" s="11">
         <v>56</v>
       </c>
-      <c r="C58" s="49"/>
+      <c r="C58" s="50"/>
       <c r="D58" s="27" t="s">
         <v>117</v>
       </c>
@@ -4788,7 +4853,7 @@
       <c r="B59" s="11">
         <v>57</v>
       </c>
-      <c r="C59" s="49"/>
+      <c r="C59" s="50"/>
       <c r="D59" s="23" t="s">
         <v>120</v>
       </c>
@@ -4809,8 +4874,8 @@
       <c r="B60" s="11">
         <v>58</v>
       </c>
-      <c r="C60" s="49"/>
-      <c r="D60" s="39" t="s">
+      <c r="C60" s="50"/>
+      <c r="D60" s="38" t="s">
         <v>122</v>
       </c>
       <c r="E60" s="2" t="s">
@@ -4825,13 +4890,13 @@
       <c r="H60" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I60" s="47"/>
+      <c r="I60" s="46"/>
     </row>
     <row r="61" spans="2:11">
       <c r="B61" s="11">
         <v>59</v>
       </c>
-      <c r="C61" s="49"/>
+      <c r="C61" s="50"/>
       <c r="D61" s="23" t="s">
         <v>124</v>
       </c>
@@ -4847,13 +4912,13 @@
       <c r="H61" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I61" s="47"/>
+      <c r="I61" s="46"/>
     </row>
     <row r="62" spans="2:11">
       <c r="B62" s="11">
         <v>60</v>
       </c>
-      <c r="C62" s="49"/>
+      <c r="C62" s="50"/>
       <c r="D62" s="23" t="s">
         <v>126</v>
       </c>
@@ -4869,13 +4934,13 @@
       <c r="H62" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I62" s="47"/>
+      <c r="I62" s="46"/>
     </row>
     <row r="63" spans="2:11">
       <c r="B63" s="11">
         <v>61</v>
       </c>
-      <c r="C63" s="49"/>
+      <c r="C63" s="50"/>
       <c r="D63" s="25" t="s">
         <v>128</v>
       </c>
@@ -4891,13 +4956,13 @@
       <c r="H63" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I63" s="47"/>
+      <c r="I63" s="46"/>
     </row>
     <row r="64" spans="2:11">
       <c r="B64" s="11">
         <v>62</v>
       </c>
-      <c r="C64" s="49"/>
+      <c r="C64" s="50"/>
       <c r="D64" s="25" t="s">
         <v>130</v>
       </c>
@@ -4907,7 +4972,7 @@
       <c r="F64" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="G64" s="42" t="s">
+      <c r="G64" s="41" t="s">
         <v>307</v>
       </c>
       <c r="H64" s="33" t="s">
@@ -4918,7 +4983,7 @@
       <c r="B65" s="11">
         <v>63</v>
       </c>
-      <c r="C65" s="49"/>
+      <c r="C65" s="50"/>
       <c r="D65" s="6" t="s">
         <v>132</v>
       </c>
@@ -4939,7 +5004,7 @@
       <c r="B66" s="11">
         <v>64</v>
       </c>
-      <c r="C66" s="49"/>
+      <c r="C66" s="50"/>
       <c r="D66" s="23" t="s">
         <v>134</v>
       </c>
@@ -4960,7 +5025,7 @@
       <c r="B67" s="11">
         <v>65</v>
       </c>
-      <c r="C67" s="49"/>
+      <c r="C67" s="50"/>
       <c r="D67" s="25" t="s">
         <v>136</v>
       </c>
@@ -5038,10 +5103,10 @@
       <c r="B3" s="11">
         <v>1</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="50" t="s">
         <v>159</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -5056,8 +5121,8 @@
       <c r="B4" s="11">
         <v>2</v>
       </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
       <c r="E4" s="8" t="s">
         <v>163</v>
       </c>
@@ -5070,8 +5135,8 @@
       <c r="B5" s="11">
         <v>3</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
       <c r="E5" s="2" t="s">
         <v>164</v>
       </c>
@@ -5084,8 +5149,8 @@
       <c r="B6" s="11">
         <v>4</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
       <c r="E6" s="2" t="s">
         <v>165</v>
       </c>
@@ -5098,8 +5163,8 @@
       <c r="B7" s="11">
         <v>5</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
       <c r="E7" s="2" t="s">
         <v>166</v>
       </c>
@@ -5112,8 +5177,8 @@
       <c r="B8" s="11">
         <v>6</v>
       </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
       <c r="E8" s="2" t="s">
         <v>167</v>
       </c>
@@ -5126,8 +5191,8 @@
       <c r="B9" s="11">
         <v>7</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
       <c r="E9" s="2" t="s">
         <v>168</v>
       </c>
@@ -5140,8 +5205,8 @@
       <c r="B10" s="11">
         <v>8</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
       <c r="E10" s="2" t="s">
         <v>169</v>
       </c>
@@ -5154,8 +5219,8 @@
       <c r="B11" s="11">
         <v>9</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
       <c r="E11" s="2" t="s">
         <v>170</v>
       </c>
@@ -5168,8 +5233,8 @@
       <c r="B12" s="11">
         <v>10</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
       <c r="E12" s="2" t="s">
         <v>171</v>
       </c>
@@ -5182,8 +5247,8 @@
       <c r="B13" s="11">
         <v>11</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
       <c r="E13" s="2" t="s">
         <v>172</v>
       </c>
@@ -5199,7 +5264,7 @@
       <c r="C14" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="D14" s="49"/>
+      <c r="D14" s="50"/>
       <c r="E14" s="2" t="s">
         <v>172</v>
       </c>
@@ -5212,10 +5277,10 @@
       <c r="B15" s="11">
         <v>13</v>
       </c>
-      <c r="C15" s="50" t="s">
+      <c r="C15" s="51" t="s">
         <v>174</v>
       </c>
-      <c r="D15" s="49"/>
+      <c r="D15" s="50"/>
       <c r="E15" s="2" t="s">
         <v>162</v>
       </c>
@@ -5228,8 +5293,8 @@
       <c r="B16" s="11">
         <v>14</v>
       </c>
-      <c r="C16" s="50"/>
-      <c r="D16" s="49"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="50"/>
       <c r="E16" s="2" t="s">
         <v>164</v>
       </c>
@@ -5242,8 +5307,8 @@
       <c r="B17" s="11">
         <v>15</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="49"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="50"/>
       <c r="E17" s="2" t="s">
         <v>168</v>
       </c>
@@ -5256,8 +5321,8 @@
       <c r="B18" s="11">
         <v>16</v>
       </c>
-      <c r="C18" s="50"/>
-      <c r="D18" s="49"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="50"/>
       <c r="E18" s="2" t="s">
         <v>170</v>
       </c>
@@ -5270,8 +5335,8 @@
       <c r="B19" s="11">
         <v>17</v>
       </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="49"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="50"/>
       <c r="E19" s="2" t="s">
         <v>172</v>
       </c>
@@ -5284,8 +5349,8 @@
       <c r="B20" s="11">
         <v>18</v>
       </c>
-      <c r="C20" s="50"/>
-      <c r="D20" s="49"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="50"/>
       <c r="E20" s="2" t="s">
         <v>175</v>
       </c>
@@ -5298,8 +5363,8 @@
       <c r="B21" s="11">
         <v>19</v>
       </c>
-      <c r="C21" s="50"/>
-      <c r="D21" s="49"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="50"/>
       <c r="E21" s="2" t="s">
         <v>176</v>
       </c>
@@ -5312,8 +5377,8 @@
       <c r="B22" s="11">
         <v>20</v>
       </c>
-      <c r="C22" s="50"/>
-      <c r="D22" s="49"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="50"/>
       <c r="E22" s="2" t="s">
         <v>177</v>
       </c>
@@ -5326,10 +5391,10 @@
       <c r="B23" s="11">
         <v>21</v>
       </c>
-      <c r="C23" s="50" t="s">
+      <c r="C23" s="51" t="s">
         <v>178</v>
       </c>
-      <c r="D23" s="49"/>
+      <c r="D23" s="50"/>
       <c r="E23" s="2" t="s">
         <v>179</v>
       </c>
@@ -5342,8 +5407,8 @@
       <c r="B24" s="11">
         <v>22</v>
       </c>
-      <c r="C24" s="50"/>
-      <c r="D24" s="49"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="50"/>
       <c r="E24" s="2" t="s">
         <v>180</v>
       </c>
@@ -5356,8 +5421,8 @@
       <c r="B25" s="11">
         <v>23</v>
       </c>
-      <c r="C25" s="50"/>
-      <c r="D25" s="49"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="50"/>
       <c r="E25" s="2" t="s">
         <v>181</v>
       </c>
@@ -5370,8 +5435,8 @@
       <c r="B26" s="11">
         <v>24</v>
       </c>
-      <c r="C26" s="50"/>
-      <c r="D26" s="49"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="50"/>
       <c r="E26" s="2" t="s">
         <v>182</v>
       </c>
@@ -5384,8 +5449,8 @@
       <c r="B27" s="11">
         <v>25</v>
       </c>
-      <c r="C27" s="50"/>
-      <c r="D27" s="49"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="50"/>
       <c r="E27" s="2" t="s">
         <v>183</v>
       </c>
@@ -5398,8 +5463,8 @@
       <c r="B28" s="11">
         <v>26</v>
       </c>
-      <c r="C28" s="50"/>
-      <c r="D28" s="49"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="50"/>
       <c r="E28" s="2" t="s">
         <v>184</v>
       </c>
@@ -5412,8 +5477,8 @@
       <c r="B29" s="11">
         <v>27</v>
       </c>
-      <c r="C29" s="50"/>
-      <c r="D29" s="49"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="50"/>
       <c r="E29" s="2" t="s">
         <v>185</v>
       </c>
@@ -5426,8 +5491,8 @@
       <c r="B30" s="11">
         <v>28</v>
       </c>
-      <c r="C30" s="50"/>
-      <c r="D30" s="49"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="50"/>
       <c r="E30" s="2" t="s">
         <v>186</v>
       </c>
@@ -5440,8 +5505,8 @@
       <c r="B31" s="11">
         <v>29</v>
       </c>
-      <c r="C31" s="50"/>
-      <c r="D31" s="49"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="50"/>
       <c r="E31" s="2" t="s">
         <v>187</v>
       </c>
@@ -5454,8 +5519,8 @@
       <c r="B32" s="11">
         <v>30</v>
       </c>
-      <c r="C32" s="50"/>
-      <c r="D32" s="49"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="50"/>
       <c r="E32" s="2" t="s">
         <v>188</v>
       </c>
@@ -5468,8 +5533,8 @@
       <c r="B33" s="11">
         <v>31</v>
       </c>
-      <c r="C33" s="50"/>
-      <c r="D33" s="49"/>
+      <c r="C33" s="51"/>
+      <c r="D33" s="50"/>
       <c r="E33" s="2" t="s">
         <v>189</v>
       </c>
@@ -5482,8 +5547,8 @@
       <c r="B34" s="11">
         <v>32</v>
       </c>
-      <c r="C34" s="50"/>
-      <c r="D34" s="49"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="50"/>
       <c r="E34" s="2" t="s">
         <v>190</v>
       </c>
@@ -5496,8 +5561,8 @@
       <c r="B35" s="11">
         <v>33</v>
       </c>
-      <c r="C35" s="50"/>
-      <c r="D35" s="49"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="50"/>
       <c r="E35" s="2" t="s">
         <v>191</v>
       </c>
@@ -5510,8 +5575,8 @@
       <c r="B36" s="11">
         <v>34</v>
       </c>
-      <c r="C36" s="50"/>
-      <c r="D36" s="49"/>
+      <c r="C36" s="51"/>
+      <c r="D36" s="50"/>
       <c r="E36" s="2" t="s">
         <v>192</v>
       </c>
@@ -5524,8 +5589,8 @@
       <c r="B37" s="11">
         <v>35</v>
       </c>
-      <c r="C37" s="50"/>
-      <c r="D37" s="49"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="50"/>
       <c r="E37" s="2" t="s">
         <v>193</v>
       </c>
@@ -5595,230 +5660,230 @@
       <c r="B3" s="33">
         <v>1</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="D3" s="42" t="s">
         <v>201</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>202</v>
       </c>
       <c r="F3" s="33"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
     </row>
     <row r="4" spans="2:9">
       <c r="B4" s="33">
         <v>2</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="43" t="s">
+      <c r="C4" s="52"/>
+      <c r="D4" s="42" t="s">
         <v>203</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="44" t="s">
         <v>204</v>
       </c>
       <c r="F4" s="33"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
     </row>
     <row r="5" spans="2:9">
       <c r="B5" s="33">
         <v>3</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="43" t="s">
+      <c r="C5" s="52"/>
+      <c r="D5" s="42" t="s">
         <v>205</v>
       </c>
-      <c r="E5" s="45" t="s">
+      <c r="E5" s="44" t="s">
         <v>206</v>
       </c>
       <c r="F5" s="33"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
     </row>
     <row r="6" spans="2:9">
       <c r="B6" s="33">
         <v>4</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="43" t="s">
+      <c r="C6" s="52"/>
+      <c r="D6" s="42" t="s">
         <v>207</v>
       </c>
-      <c r="E6" s="45" t="s">
+      <c r="E6" s="44" t="s">
         <v>208</v>
       </c>
       <c r="F6" s="33"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
     </row>
     <row r="7" spans="2:9">
       <c r="B7" s="33">
         <v>5</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="43" t="s">
+      <c r="C7" s="52"/>
+      <c r="D7" s="42" t="s">
         <v>209</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="44" t="s">
         <v>210</v>
       </c>
       <c r="F7" s="33"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
     </row>
     <row r="8" spans="2:9">
       <c r="B8" s="33">
         <v>6</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="43" t="s">
+      <c r="C8" s="52"/>
+      <c r="D8" s="42" t="s">
         <v>211</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>212</v>
       </c>
       <c r="F8" s="33"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
     </row>
     <row r="9" spans="2:9">
       <c r="B9" s="33">
         <v>7</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="42" t="s">
         <v>211</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>212</v>
       </c>
       <c r="F9" s="33"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
     </row>
     <row r="10" spans="2:9">
       <c r="B10" s="33">
         <v>8</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="43" t="s">
+      <c r="C10" s="52"/>
+      <c r="D10" s="42" t="s">
         <v>213</v>
       </c>
-      <c r="E10" s="45" t="s">
+      <c r="E10" s="44" t="s">
         <v>214</v>
       </c>
       <c r="F10" s="33"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
     </row>
     <row r="11" spans="2:9">
       <c r="B11" s="33">
         <v>9</v>
       </c>
-      <c r="C11" s="51"/>
-      <c r="D11" s="43" t="s">
+      <c r="C11" s="52"/>
+      <c r="D11" s="42" t="s">
         <v>215</v>
       </c>
-      <c r="E11" s="45" t="s">
+      <c r="E11" s="44" t="s">
         <v>216</v>
       </c>
       <c r="F11" s="33"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
     </row>
     <row r="12" spans="2:9">
       <c r="B12" s="33">
         <v>10</v>
       </c>
-      <c r="C12" s="51"/>
-      <c r="D12" s="43" t="s">
+      <c r="C12" s="52"/>
+      <c r="D12" s="42" t="s">
         <v>217</v>
       </c>
-      <c r="E12" s="45" t="s">
+      <c r="E12" s="44" t="s">
         <v>218</v>
       </c>
       <c r="F12" s="33"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="44"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
     </row>
     <row r="13" spans="2:9">
       <c r="B13" s="33">
         <v>11</v>
       </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="43" t="s">
+      <c r="C13" s="52"/>
+      <c r="D13" s="42" t="s">
         <v>219</v>
       </c>
-      <c r="E13" s="45" t="s">
+      <c r="E13" s="44" t="s">
         <v>220</v>
       </c>
       <c r="F13" s="33"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
     </row>
     <row r="14" spans="2:9">
       <c r="B14" s="33">
         <v>12</v>
       </c>
-      <c r="C14" s="51"/>
-      <c r="D14" s="43" t="s">
+      <c r="C14" s="52"/>
+      <c r="D14" s="42" t="s">
         <v>221</v>
       </c>
-      <c r="E14" s="45" t="s">
+      <c r="E14" s="44" t="s">
         <v>222</v>
       </c>
       <c r="F14" s="33"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
     </row>
     <row r="15" spans="2:9">
       <c r="B15" s="33">
         <v>13</v>
       </c>
-      <c r="C15" s="51"/>
-      <c r="D15" s="43" t="s">
+      <c r="C15" s="52"/>
+      <c r="D15" s="42" t="s">
         <v>223</v>
       </c>
-      <c r="E15" s="45" t="s">
+      <c r="E15" s="44" t="s">
         <v>224</v>
       </c>
       <c r="F15" s="33"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
     </row>
     <row r="16" spans="2:9">
       <c r="B16" s="33">
         <v>14</v>
       </c>
-      <c r="C16" s="51"/>
-      <c r="D16" s="43" t="s">
+      <c r="C16" s="52"/>
+      <c r="D16" s="42" t="s">
         <v>225</v>
       </c>
-      <c r="E16" s="45" t="s">
+      <c r="E16" s="44" t="s">
         <v>226</v>
       </c>
       <c r="F16" s="33"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="44"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
     </row>
     <row r="17" spans="2:9">
       <c r="B17" s="33">
         <v>15</v>
       </c>
-      <c r="C17" s="51"/>
-      <c r="D17" s="43" t="s">
+      <c r="C17" s="52"/>
+      <c r="D17" s="42" t="s">
         <v>227</v>
       </c>
-      <c r="E17" s="45" t="s">
+      <c r="E17" s="44" t="s">
         <v>228</v>
       </c>
       <c r="F17" s="33"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>